<commit_message>
Add a 2nd worksheet to clippy.xls[x]
Should be a good example for #492
</commit_message>
<xml_diff>
--- a/inst/extdata/clippy.xlsx
+++ b/inst/extdata/clippy.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/rrr/readxl/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{81F69A64-2982-C446-A50C-FAADD4C4626D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="list-column" sheetId="1" r:id="rId1"/>
+    <sheet name="two-row-header" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -51,12 +53,33 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>death</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>(in grams)</t>
+  </si>
+  <si>
+    <t>(office supply type)</t>
+  </si>
+  <si>
+    <t>(at birth)</t>
+  </si>
+  <si>
+    <t>(date is approximate)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -98,6 +121,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -365,11 +391,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,4 +443,61 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF597CD1-05A9-FA40-8B6A-50B15ADE0850}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>39083</v>
+      </c>
+      <c r="D3">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>